<commit_message>
Refactored Folders and Files
</commit_message>
<xml_diff>
--- a/notebooks/Image-Similarity/Similarity.xlsx
+++ b/notebooks/Image-Similarity/Similarity.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,149 +452,44 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.4745</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Dog-2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>shutterstock_513244762</t>
+          <t>Dog-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.4517</v>
+        <v>0.541</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Dog-2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dog-1</t>
+          <t>Cat-1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.4438</v>
+        <v>0.5494</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Dog-1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>Cat-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0.4376</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Dog-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0.7052</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>shutterstock_513244762</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Dog-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0.5992</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>shutterstock_513244762</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Dog-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>0.547</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>shutterstock_513244762</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Cat-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>0.5669999999999999</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Dog-2</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Dog-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>0.541</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Dog-2</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Cat-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>0.5494</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Dog-1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
         <is>
           <t>Cat-1</t>
         </is>

</xml_diff>